<commit_message>
Matriz de riesgos actualizada
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Proyecto/Matriz_de_Riesgos.xlsx
+++ b/Fase 1/Evidencias Proyecto/Matriz_de_Riesgos.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basty\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CETECOM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2E7F69-D33B-4577-A6AA-1E02802649EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA7347E-35FD-4EFB-A2AB-0C33E1B8C337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Riesgos" sheetId="1" r:id="rId1"/>
+    <sheet name="Matriz" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Riesgos!$A$1:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Riesgos!$B$1:$H$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>Riesgo</t>
   </si>
@@ -140,15 +139,6 @@
     <t>Uso de herramientas de gestión de tareas y reuniones periódicas.</t>
   </si>
   <si>
-    <t>Nivel de riesgo</t>
-  </si>
-  <si>
-    <t>Impacto (1 - 5)</t>
-  </si>
-  <si>
-    <t>Probabilidad (1 - 5)</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -179,17 +169,50 @@
     <t>Baja</t>
   </si>
   <si>
-    <t>Media-Alta</t>
-  </si>
-  <si>
     <t>Media</t>
+  </si>
+  <si>
+    <t>IMPACTO</t>
+  </si>
+  <si>
+    <t>ALTO</t>
+  </si>
+  <si>
+    <t>MEDIO</t>
+  </si>
+  <si>
+    <t>BAJO</t>
+  </si>
+  <si>
+    <t>OCURRENCIA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Impacto (1 - 3)</t>
+  </si>
+  <si>
+    <t>1,2,5</t>
+  </si>
+  <si>
+    <t>Ocurrencia (1 - 3)</t>
+  </si>
+  <si>
+    <t>3,4,10</t>
+  </si>
+  <si>
+    <t>7,9,11</t>
+  </si>
+  <si>
+    <t>Numeros = ID riesgo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,8 +228,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,8 +264,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -273,11 +354,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -289,27 +444,53 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCD6F6D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCD6F6D"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <font>
         <strike val="0"/>
@@ -357,6 +538,118 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFA6D86E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCD6F6D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7C971"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA6D86E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCD6F6D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7C971"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA6D86E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCD6F6D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC7C971"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA6D86E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCD6F6D"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCD6F6D"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -381,9 +674,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -421,9 +714,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -456,9 +749,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -491,9 +801,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -669,40 +996,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H316"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="110.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="110.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>15</v>
@@ -711,187 +1037,180 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <f>IF(C2*D2&lt;10, "Bajo", IF(C2*D2&lt;=18, "Medio", "Alto"))</f>
-        <v>Alto</v>
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <f>IF(C3*D3&lt;10, "Bajo", IF(C3*D3&lt;=18, "Medio", "Alto"))</f>
-        <v>Medio</v>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>4</v>
-      </c>
-      <c r="E4" s="1" t="str">
-        <f>IF(C4*D4&lt;10, "Bajo", IF(C4*D4&lt;=18, "Medio", "Alto"))</f>
-        <v>Medio</v>
+      <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="str">
-        <f>IF(C5*D5&lt;10, "Bajo", IF(C5*D5&lt;=18, "Medio", "Alto"))</f>
-        <v>Medio</v>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="str">
-        <f>IF(C6*D6&lt;10, "Bajo", IF(C6*D6&lt;=18, "Medio", "Alto"))</f>
-        <v>Medio</v>
+      <c r="D6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f>IF(C7*D7&lt;10, "Bajo", IF(C7*D7&lt;=18, "Medio", "Alto"))</f>
-        <v>Medio</v>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="str">
-        <f>IF(C8*D8&lt;10, "Bajo", IF(C8*D8&lt;=18, "Medio", "Alto"))</f>
-        <v>Bajo</v>
+      <c r="E8" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>17</v>
@@ -900,25 +1219,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>4</v>
-      </c>
-      <c r="E9" s="1" t="str">
-        <f>IF(C9*D9&lt;10, "Bajo", IF(C9*D9&lt;=18, "Medio", "Alto"))</f>
-        <v>Bajo</v>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>17</v>
@@ -927,25 +1245,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1" t="str">
-        <f>IF(C10*D10&lt;10, "Bajo", IF(C10*D10&lt;=18, "Medio", "Alto"))</f>
-        <v>Bajo</v>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>17</v>
@@ -954,25 +1271,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="1">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1">
-        <v>4</v>
-      </c>
-      <c r="E11" s="1" t="str">
-        <f>IF(C11*D11&lt;10, "Bajo", IF(C11*D11&lt;=18, "Medio", "Alto"))</f>
-        <v>Medio</v>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>16</v>
@@ -981,25 +1297,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1">
-        <v>3</v>
-      </c>
-      <c r="E12" s="1" t="str">
-        <f>IF(C12*D12&lt;10, "Bajo", IF(C12*D12&lt;=18, "Medio", "Alto"))</f>
-        <v>Bajo</v>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>16</v>
@@ -1008,49 +1323,208 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="316" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B316" t="s">
-        <v>37</v>
+    <row r="316" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C316" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H12">
-      <sortCondition sortBy="cellColor" ref="E1:E12" dxfId="1"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="D1 E2:F2 F3:F7 F11:F12 C14:C1048576">
-    <cfRule type="containsText" dxfId="7" priority="19" operator="containsText" text="Bajo">
-      <formula>NOT(ISERROR(SEARCH("Bajo",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="20" operator="containsText" text="Medio">
-      <formula>NOT(ISERROR(SEARCH("Medio",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="21" operator="containsText" text="Alto">
-      <formula>NOT(ISERROR(SEARCH("Alto",C1)))</formula>
+  <autoFilter ref="B1:H12" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="E1 D14:D1048576 F2:F7 F11:F12">
+    <cfRule type="containsText" dxfId="17" priority="33" operator="containsText" text="Bajo">
+      <formula>NOT(ISERROR(SEARCH("Bajo",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="34" operator="containsText" text="Medio">
+      <formula>NOT(ISERROR(SEARCH("Medio",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="35" operator="containsText" text="Alto">
+      <formula>NOT(ISERROR(SEARCH("Alto",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E13">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Bajo">
-      <formula>NOT(ISERROR(SEARCH("Bajo",E3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Medio">
-      <formula>NOT(ISERROR(SEARCH("Medio",E3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="Alto">
-      <formula>NOT(ISERROR(SEARCH("Alto",E3)))</formula>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Alta">
+      <formula>NOT(ISERROR(SEARCH("Alta",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="Media">
+      <formula>NOT(ISERROR(SEARCH("Media",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Bajo">
+      <formula>NOT(ISERROR(SEARCH("Bajo",F8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Medio">
+      <formula>NOT(ISERROR(SEARCH("Medio",F8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Alto">
+      <formula>NOT(ISERROR(SEARCH("Alto",F8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Bajo">
+      <formula>NOT(ISERROR(SEARCH("Bajo",F9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Medio">
+      <formula>NOT(ISERROR(SEARCH("Medio",F9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Alto">
+      <formula>NOT(ISERROR(SEARCH("Alto",F9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Bajo">
+      <formula>NOT(ISERROR(SEARCH("Bajo",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Medio">
+      <formula>NOT(ISERROR(SEARCH("Medio",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Alto">
+      <formula>NOT(ISERROR(SEARCH("Alto",F10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Bajo">
+      <formula>NOT(ISERROR(SEARCH("Bajo",F12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Medio">
+      <formula>NOT(ISERROR(SEARCH("Medio",F12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Alto">
+      <formula>NOT(ISERROR(SEARCH("Alto",F12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF00FAE2-D0F1-4615-9835-F6FBC2FC4465}">
+  <dimension ref="A1:R37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="11.5546875" style="8"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="8" max="18" width="11.5546875" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="3:7" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="3:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="9">
+        <v>8</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="14"/>
+      <c r="D5" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="3:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="19"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="3:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="E8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>